<commit_message>
small  but important fix
</commit_message>
<xml_diff>
--- a/HW3/results_test1.xlsx
+++ b/HW3/results_test1.xlsx
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -771,34 +771,34 @@
         <v>2</v>
       </c>
       <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>3</v>
+      </c>
+      <c r="F2" s="22">
         <v>5</v>
       </c>
-      <c r="E2" s="22">
+      <c r="G2" s="22">
         <v>7</v>
       </c>
-      <c r="F2" s="22">
+      <c r="H2" s="22">
         <v>9</v>
       </c>
-      <c r="G2" s="22">
+      <c r="I2" s="22">
         <v>11</v>
       </c>
-      <c r="H2" s="22">
+      <c r="J2" s="22">
         <v>13</v>
       </c>
-      <c r="I2" s="22">
+      <c r="K2" s="22">
         <v>15</v>
       </c>
-      <c r="J2" s="22">
+      <c r="L2" s="22">
         <v>17</v>
       </c>
-      <c r="K2" s="22">
+      <c r="M2" s="23">
         <v>19</v>
-      </c>
-      <c r="L2" s="22">
-        <v>21</v>
-      </c>
-      <c r="M2" s="23">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -812,31 +812,35 @@
         <v>3</v>
       </c>
       <c r="D3" s="9">
-        <v>0.85609756097560896</v>
+        <v>0.75121951219512195</v>
       </c>
       <c r="E3" s="10">
-        <v>0.86036585365853602</v>
+        <v>0.81036585365853597</v>
       </c>
       <c r="F3" s="10">
-        <v>0.86158536585365797</v>
+        <v>0.83780487804878001</v>
       </c>
       <c r="G3" s="10">
-        <v>0.86158536585365797</v>
+        <v>0.85243902439024299</v>
       </c>
       <c r="H3" s="10">
-        <v>0.86158536585365797</v>
+        <v>0.85365853658536595</v>
       </c>
       <c r="I3" s="10">
-        <v>0.86158536585365797</v>
+        <v>0.85731707317073103</v>
       </c>
       <c r="J3" s="10">
-        <v>0.86158536585365797</v>
+        <v>0.85975609756097504</v>
       </c>
       <c r="K3" s="10">
         <v>0.86158536585365797</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
+      <c r="L3" s="10">
+        <v>0.86219512195121895</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.86280487804878003</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -847,27 +851,35 @@
         <v>4</v>
       </c>
       <c r="D4" s="14">
-        <v>0.86158536585365797</v>
+        <v>0.86185574699783696</v>
       </c>
       <c r="E4" s="15">
-        <v>0.86158536585365797</v>
+        <v>0.86002088461251502</v>
       </c>
       <c r="F4" s="15">
-        <v>0.86158536585365797</v>
+        <v>0.86002088461251502</v>
       </c>
       <c r="G4" s="15">
-        <v>0.86158536585365797</v>
+        <v>0.86002088461251502</v>
       </c>
       <c r="H4" s="15">
-        <v>0.86158536585365797</v>
+        <v>0.86002088461251502</v>
       </c>
       <c r="I4" s="15">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
+        <v>0.86002088461251502</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0.86002088461251502</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0.86002088461251502</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0.86002088461251502</v>
+      </c>
+      <c r="M4" s="16">
+        <v>0.86002088461251502</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -877,24 +889,12 @@
       <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="14">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="F5" s="15">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="H5" s="15">
-        <v>0.86158536585365797</v>
-      </c>
-      <c r="I5" s="15">
-        <v>0.86158536585365797</v>
-      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -908,36 +908,16 @@
       <c r="C6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14">
-        <v>0.91156671887819696</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.91034068024166404</v>
-      </c>
-      <c r="F6" s="15">
-        <v>0.91522525546356304</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.91307898858805103</v>
-      </c>
-      <c r="H6" s="15">
-        <v>0.91674498396360105</v>
-      </c>
-      <c r="I6" s="15">
-        <v>0.90942604609532296</v>
-      </c>
-      <c r="J6" s="15">
-        <v>0.91980029089281701</v>
-      </c>
-      <c r="K6" s="15">
-        <v>0.91522152606847096</v>
-      </c>
-      <c r="L6" s="15">
-        <v>0.92498415007085799</v>
-      </c>
-      <c r="M6" s="16">
-        <v>0.91217647497575904</v>
-      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -947,36 +927,16 @@
       <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="14">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="I7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="J7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="K7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="M7" s="16">
-        <v>0.86003393749533796</v>
-      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -986,36 +946,16 @@
       <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="18">
-        <v>0.86094857164167904</v>
-      </c>
-      <c r="E8" s="19">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="F8" s="19">
-        <v>0.86064369359289905</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0.86033881554411795</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0.86125344969046003</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0.86003393749533796</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0.86033881554411795</v>
-      </c>
-      <c r="M8" s="20">
-        <v>0.86003393749533796</v>
-      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1028,29 +968,35 @@
         <v>3</v>
       </c>
       <c r="D9" s="24">
-        <v>0.88548472748783302</v>
+        <v>0.64715909090908996</v>
       </c>
       <c r="E9" s="25">
-        <v>0.90922686268183095</v>
+        <v>0.803367582210749</v>
       </c>
       <c r="F9" s="25">
-        <v>0.92394430104057401</v>
+        <v>0.76006964050442305</v>
       </c>
       <c r="G9" s="25">
-        <v>0.93816649189320001</v>
+        <v>0.78319637143394905</v>
       </c>
       <c r="H9" s="25">
-        <v>0.94299023957409001</v>
+        <v>0.89612002903928301</v>
       </c>
       <c r="I9" s="25">
-        <v>0.95065556855153099</v>
+        <v>0.91108248635422495</v>
       </c>
       <c r="J9" s="25">
-        <v>0.95844609582963602</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="26"/>
+        <v>0.92060293484982902</v>
+      </c>
+      <c r="K9" s="25">
+        <v>0.93049679357909099</v>
+      </c>
+      <c r="L9" s="25">
+        <v>0.93235107284020302</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0.94088640396870205</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -1061,26 +1007,32 @@
         <v>4</v>
       </c>
       <c r="D10" s="14">
-        <v>0.88511215751122596</v>
+        <v>0.73003229948105697</v>
       </c>
       <c r="E10" s="15">
-        <v>0.91145270361108799</v>
+        <v>0.80744501357855303</v>
       </c>
       <c r="F10" s="15">
-        <v>0.92752950982764604</v>
+        <v>0.76019349439380501</v>
       </c>
       <c r="G10" s="15">
-        <v>0.93655739963969697</v>
+        <v>0.87187760479685905</v>
       </c>
       <c r="H10" s="15">
-        <v>0.94805934231400002</v>
+        <v>0.88993540103788504</v>
       </c>
       <c r="I10" s="15">
-        <v>0.95312945336237198</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+        <v>0.90996763329837804</v>
+      </c>
+      <c r="J10" s="15">
+        <v>0.91615108493990405</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.92184080153800596</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.93717885375494003</v>
+      </c>
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1091,24 +1043,12 @@
       <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="14">
-        <v>0.89117141916054898</v>
-      </c>
-      <c r="E11" s="15">
-        <v>0.91034053937780601</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0.92084997042295103</v>
-      </c>
-      <c r="G11" s="15">
-        <v>0.93804499072356196</v>
-      </c>
-      <c r="H11" s="15">
-        <v>0.94496618805624999</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0.951521201365921</v>
-      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1122,36 +1062,16 @@
       <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="14">
-        <v>0.88486360947540998</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0.90860944180043501</v>
-      </c>
-      <c r="F12" s="15">
-        <v>0.92617098222688199</v>
-      </c>
-      <c r="G12" s="15">
-        <v>0.943237107095802</v>
-      </c>
-      <c r="H12" s="15">
-        <v>0.95040819687558797</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0.95226432470221301</v>
-      </c>
-      <c r="J12" s="15">
-        <v>0.96005653249442002</v>
-      </c>
-      <c r="K12" s="15">
-        <v>0.96215801538006496</v>
-      </c>
-      <c r="L12" s="15">
-        <v>0.96722795837702602</v>
-      </c>
-      <c r="M12" s="16">
-        <v>0.96660868893011698</v>
-      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -1161,36 +1081,16 @@
       <c r="C13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="14">
-        <v>0.88275842945873995</v>
-      </c>
-      <c r="E13" s="15">
-        <v>0.91133002608157798</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0.92901390793471506</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0.93940217391304304</v>
-      </c>
-      <c r="H13" s="15">
-        <v>0.95139751552795004</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0.95275839584845801</v>
-      </c>
-      <c r="J13" s="15">
-        <v>0.95881816165201195</v>
-      </c>
-      <c r="K13" s="15">
-        <v>0.95795219273480103</v>
-      </c>
-      <c r="L13" s="15">
-        <v>0.96685639670888102</v>
-      </c>
-      <c r="M13" s="16">
-        <v>0.96920609152752002</v>
-      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1200,36 +1100,16 @@
       <c r="C14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="18">
-        <v>0.88585679331020895</v>
-      </c>
-      <c r="E14" s="19">
-        <v>0.90848373934554005</v>
-      </c>
-      <c r="F14" s="19">
-        <v>0.92282995213895802</v>
-      </c>
-      <c r="G14" s="19">
-        <v>0.94064088085827202</v>
-      </c>
-      <c r="H14" s="19">
-        <v>0.94521540829770601</v>
-      </c>
-      <c r="I14" s="19">
-        <v>0.950284174934796</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0.96203399343927198</v>
-      </c>
-      <c r="K14" s="19">
-        <v>0.87434039821462095</v>
-      </c>
-      <c r="L14" s="19">
-        <v>0.96797040950767599</v>
-      </c>
-      <c r="M14" s="20">
-        <v>0.96722779032561601</v>
-      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>